<commit_message>
Add seed construction and pseudodata generator to RaCA-SOC-a main file. Restructure endmember worksheet to include plots of each spectrum.
</commit_message>
<xml_diff>
--- a/data/Soil endmember mastersheet.xlsx
+++ b/data/Soil endmember mastersheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ecoleman/Documents/RaCA-SOC-a-spectrum-analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360A005B-2A78-4442-A1D4-EBDFAF384318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{135BFAB7-DFF4-8943-8321-35E89D918779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="34400" windowHeight="28300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="USGS_spectra" sheetId="1" r:id="rId1"/>
@@ -19909,7 +19909,7 @@
   </sheetPr>
   <dimension ref="A1:O155"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C113" sqref="C113"/>
     </sheetView>
@@ -29445,9 +29445,9 @@
   </sheetPr>
   <dimension ref="A1:V12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29510,7 +29510,7 @@
       <c r="B3" s="4" t="s">
         <v>382</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="24" t="s">
         <v>383</v>
       </c>
       <c r="E3" s="4" t="s">
@@ -29524,7 +29524,7 @@
       <c r="B4" s="4" t="s">
         <v>385</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="24" t="s">
         <v>386</v>
       </c>
       <c r="E4" s="4" t="s">
@@ -29538,7 +29538,7 @@
       <c r="B5" s="4" t="s">
         <v>388</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="24" t="s">
         <v>389</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -29552,7 +29552,7 @@
       <c r="B6" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="24" t="s">
         <v>392</v>
       </c>
       <c r="E6" s="4" t="s">
@@ -29566,7 +29566,7 @@
       <c r="B7" s="4" t="s">
         <v>394</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="C7" s="24" t="s">
         <v>395</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -29580,7 +29580,7 @@
       <c r="B8" s="4" t="s">
         <v>397</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="24" t="s">
         <v>398</v>
       </c>
       <c r="E8" s="4" t="s">

</xml_diff>